<commit_message>
lagt til vurdert dato
</commit_message>
<xml_diff>
--- a/ExampleIG/output/StructureDefinition-hn-basis-serviceRequest.xlsx
+++ b/ExampleIG/output/StructureDefinition-hn-basis-serviceRequest.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-28T17:18:13+02:00</t>
+    <t>2025-09-29T11:26:30+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -509,10 +509,10 @@
 </t>
   </si>
   <si>
-    <t>Dato for frist for vurdering</t>
-  </si>
-  <si>
-    <t>Dato for frist for vurdering.</t>
+    <t>Vurdert dato</t>
+  </si>
+  <si>
+    <t>Brukes når forespørsel er vurdert og/eller henvisning er avvist/avsluttet.</t>
   </si>
   <si>
     <t>ServiceRequest.extension:statusReason</t>

</xml_diff>